<commit_message>
scripts, data, and labwork folder moving from archive
</commit_message>
<xml_diff>
--- a/data/01_QC/bismark_statistics.xlsx
+++ b/data/01_QC/bismark_statistics.xlsx
@@ -1,31 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\BoxDrive\Box\Science\Fisheries\Projects\Epigenetic Aging\github\Epigenetic_aging_haddock\data\01_QC\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A67870CE-AE55-4B0D-9DF5-FB3C1AE637D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D14E675C-6290-44E9-8AF4-26F003583EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="statistics" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="152">
   <si>
     <t>Sample Name</t>
   </si>
@@ -466,6 +477,21 @@
   </si>
   <si>
     <t>Duplicates (%)</t>
+  </si>
+  <si>
+    <t>Average aligned %</t>
+  </si>
+  <si>
+    <t>Average mCpG %</t>
+  </si>
+  <si>
+    <t>Average Cytosines</t>
+  </si>
+  <si>
+    <t>Total meth</t>
+  </si>
+  <si>
+    <t>Average total meth</t>
   </si>
 </sst>
 </file>
@@ -473,10 +499,18 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="170" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -504,9 +538,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -787,10 +823,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G141"/>
+  <dimension ref="A1:N141"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -799,9 +835,13 @@
     <col min="2" max="5" width="16.77734375" customWidth="1"/>
     <col min="6" max="6" width="14.44140625" customWidth="1"/>
     <col min="7" max="7" width="14.5546875" customWidth="1"/>
+    <col min="9" max="10" width="12.5546875" customWidth="1"/>
+    <col min="12" max="12" width="10.6640625" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -823,8 +863,11 @@
       <c r="G1" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -846,8 +889,23 @@
       <c r="G2" s="1">
         <v>0.40100000000000002</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I2" s="1">
+        <f>SUM(B2:D2)</f>
+        <v>0.74</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="M2" s="2">
+        <f>AVERAGE(F2:F500)*100</f>
+        <v>44.125000000000007</v>
+      </c>
+      <c r="N2" s="2">
+        <f>_xlfn.STDEV.S(G2:G300)/SQRT(COUNT(G2:G300))*100</f>
+        <v>0.38876427262312002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -869,8 +927,23 @@
       <c r="G3" s="1">
         <v>0.32400000000000001</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I3" s="1">
+        <f t="shared" ref="I3:I66" si="0">SUM(B3:D3)</f>
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="M3" s="2">
+        <f>AVERAGE(B2:B501)*100</f>
+        <v>64.731428571428594</v>
+      </c>
+      <c r="N3" s="2">
+        <f>_xlfn.STDEV.S(B2:B501)/SQRT(COUNT(B2:B500))*100</f>
+        <v>0.10593917913371287</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -892,8 +965,23 @@
       <c r="G4" s="1">
         <v>0.254</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I4" s="1">
+        <f t="shared" si="0"/>
+        <v>0.79700000000000004</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="M4" s="2">
+        <f>AVERAGE(E2:E502)</f>
+        <v>1139.187857142857</v>
+      </c>
+      <c r="N4" s="2">
+        <f>_xlfn.STDEV.S(E2:E502)/SQRT(COUNT(E2:E501))</f>
+        <v>26.651114611567504</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -915,8 +1003,12 @@
       <c r="G5" s="1">
         <v>0.36299999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I5" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76400000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -938,8 +1030,23 @@
       <c r="G6" s="1">
         <v>0.42199999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I6" s="1">
+        <f t="shared" si="0"/>
+        <v>0.69599999999999995</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="M6" s="2">
+        <f>AVERAGE(I2:I504)*100</f>
+        <v>76.055714285714345</v>
+      </c>
+      <c r="N6" s="2">
+        <f>_xlfn.STDEV.S(I2:I504)/SQRT(COUNT(I5:I503))*100</f>
+        <v>0.25571300683950887</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -961,8 +1068,12 @@
       <c r="G7" s="1">
         <v>0.27300000000000002</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I7" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75800000000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -984,8 +1095,12 @@
       <c r="G8" s="1">
         <v>0.30399999999999999</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I8" s="1">
+        <f t="shared" si="0"/>
+        <v>0.80500000000000005</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -1007,8 +1122,12 @@
       <c r="G9" s="1">
         <v>0.25600000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I9" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1030,8 +1149,12 @@
       <c r="G10" s="1">
         <v>0.251</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I10" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77200000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -1053,8 +1176,12 @@
       <c r="G11" s="1">
         <v>0.28799999999999998</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I11" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>11</v>
       </c>
@@ -1076,8 +1203,12 @@
       <c r="G12" s="1">
         <v>0.27900000000000003</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I12" s="1">
+        <f t="shared" si="0"/>
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>12</v>
       </c>
@@ -1099,8 +1230,12 @@
       <c r="G13" s="1">
         <v>0.29599999999999999</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I13" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76500000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>13</v>
       </c>
@@ -1122,8 +1257,12 @@
       <c r="G14" s="1">
         <v>0.32600000000000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I14" s="1">
+        <f t="shared" si="0"/>
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>14</v>
       </c>
@@ -1145,8 +1284,12 @@
       <c r="G15" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I15" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>15</v>
       </c>
@@ -1168,8 +1311,12 @@
       <c r="G16" s="1">
         <v>0.41699999999999998</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I16" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>16</v>
       </c>
@@ -1191,8 +1338,12 @@
       <c r="G17" s="1">
         <v>0.26800000000000002</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I17" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77500000000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>17</v>
       </c>
@@ -1214,8 +1365,12 @@
       <c r="G18" s="1">
         <v>0.30499999999999999</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I18" s="1">
+        <f t="shared" si="0"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>18</v>
       </c>
@@ -1237,8 +1392,12 @@
       <c r="G19" s="1">
         <v>0.38300000000000001</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>19</v>
       </c>
@@ -1260,8 +1419,12 @@
       <c r="G20" s="1">
         <v>0.375</v>
       </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>20</v>
       </c>
@@ -1283,8 +1446,12 @@
       <c r="G21" s="1">
         <v>0.39900000000000002</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.78400000000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>21</v>
       </c>
@@ -1306,8 +1473,12 @@
       <c r="G22" s="1">
         <v>0.32700000000000001</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>22</v>
       </c>
@@ -1329,8 +1500,12 @@
       <c r="G23" s="1">
         <v>0.31900000000000001</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.7350000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>23</v>
       </c>
@@ -1352,8 +1527,12 @@
       <c r="G24" s="1">
         <v>0.33200000000000002</v>
       </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I24" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72199999999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>24</v>
       </c>
@@ -1375,8 +1554,12 @@
       <c r="G25" s="1">
         <v>0.35099999999999998</v>
       </c>
-    </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I25" s="1">
+        <f t="shared" si="0"/>
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>25</v>
       </c>
@@ -1398,8 +1581,12 @@
       <c r="G26" s="1">
         <v>0.38300000000000001</v>
       </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I26" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73000000000000009</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>26</v>
       </c>
@@ -1421,8 +1608,12 @@
       <c r="G27" s="1">
         <v>0.38300000000000001</v>
       </c>
-    </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I27" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>27</v>
       </c>
@@ -1444,8 +1635,12 @@
       <c r="G28" s="1">
         <v>0.39500000000000002</v>
       </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I28" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73299999999999998</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>28</v>
       </c>
@@ -1467,8 +1662,12 @@
       <c r="G29" s="1">
         <v>0.34599999999999997</v>
       </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I29" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>29</v>
       </c>
@@ -1490,8 +1689,12 @@
       <c r="G30" s="1">
         <v>0.29399999999999998</v>
       </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I30" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>30</v>
       </c>
@@ -1513,8 +1716,12 @@
       <c r="G31" s="1">
         <v>0.30499999999999999</v>
       </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I31" s="1">
+        <f t="shared" si="0"/>
+        <v>0.746</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>31</v>
       </c>
@@ -1536,8 +1743,12 @@
       <c r="G32" s="1">
         <v>0.33400000000000002</v>
       </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I32" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>32</v>
       </c>
@@ -1559,8 +1770,12 @@
       <c r="G33" s="1">
         <v>0.30099999999999999</v>
       </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I33" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71699999999999997</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>33</v>
       </c>
@@ -1582,8 +1797,12 @@
       <c r="G34" s="1">
         <v>0.30399999999999999</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I34" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74099999999999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>34</v>
       </c>
@@ -1605,8 +1824,12 @@
       <c r="G35" s="1">
         <v>0.34200000000000003</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I35" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>35</v>
       </c>
@@ -1628,8 +1851,12 @@
       <c r="G36" s="1">
         <v>0.27</v>
       </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I36" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>36</v>
       </c>
@@ -1651,8 +1878,12 @@
       <c r="G37" s="1">
         <v>0.34799999999999998</v>
       </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I37" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>37</v>
       </c>
@@ -1674,8 +1905,12 @@
       <c r="G38" s="1">
         <v>0.435</v>
       </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I38" s="1">
+        <f t="shared" si="0"/>
+        <v>0.755</v>
+      </c>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>38</v>
       </c>
@@ -1697,8 +1932,12 @@
       <c r="G39" s="1">
         <v>0.255</v>
       </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I39" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72900000000000009</v>
+      </c>
+    </row>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>39</v>
       </c>
@@ -1720,8 +1959,12 @@
       <c r="G40" s="1">
         <v>0.314</v>
       </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I40" s="1">
+        <f t="shared" si="0"/>
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>40</v>
       </c>
@@ -1743,8 +1986,12 @@
       <c r="G41" s="1">
         <v>0.27700000000000002</v>
       </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I41" s="1">
+        <f t="shared" si="0"/>
+        <v>0.751</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>41</v>
       </c>
@@ -1766,8 +2013,12 @@
       <c r="G42" s="1">
         <v>0.311</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I42" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71599999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>42</v>
       </c>
@@ -1789,8 +2040,12 @@
       <c r="G43" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I43" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>43</v>
       </c>
@@ -1812,8 +2067,12 @@
       <c r="G44" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I44" s="1">
+        <f t="shared" si="0"/>
+        <v>0.7350000000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>44</v>
       </c>
@@ -1835,8 +2094,12 @@
       <c r="G45" s="1">
         <v>0.318</v>
       </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I45" s="1">
+        <f t="shared" si="0"/>
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>45</v>
       </c>
@@ -1858,8 +2121,12 @@
       <c r="G46" s="1">
         <v>0.26200000000000001</v>
       </c>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I46" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74399999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>46</v>
       </c>
@@ -1881,8 +2148,12 @@
       <c r="G47" s="1">
         <v>0.27700000000000002</v>
       </c>
-    </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I47" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>47</v>
       </c>
@@ -1904,8 +2175,12 @@
       <c r="G48" s="1">
         <v>0.30399999999999999</v>
       </c>
-    </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I48" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>48</v>
       </c>
@@ -1927,8 +2202,12 @@
       <c r="G49" s="1">
         <v>0.38</v>
       </c>
-    </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I49" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71399999999999997</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>49</v>
       </c>
@@ -1950,8 +2229,12 @@
       <c r="G50" s="1">
         <v>0.35099999999999998</v>
       </c>
-    </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I50" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72500000000000009</v>
+      </c>
+    </row>
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>50</v>
       </c>
@@ -1973,8 +2256,12 @@
       <c r="G51" s="1">
         <v>0.34699999999999998</v>
       </c>
-    </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I51" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74299999999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>51</v>
       </c>
@@ -1996,8 +2283,12 @@
       <c r="G52" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I52" s="1">
+        <f t="shared" si="0"/>
+        <v>0.76300000000000001</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
         <v>52</v>
       </c>
@@ -2019,8 +2310,12 @@
       <c r="G53" s="1">
         <v>0.34100000000000003</v>
       </c>
-    </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I53" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>53</v>
       </c>
@@ -2042,8 +2337,12 @@
       <c r="G54" s="1">
         <v>0.30499999999999999</v>
       </c>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I54" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72899999999999998</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>54</v>
       </c>
@@ -2065,8 +2364,12 @@
       <c r="G55" s="1">
         <v>0.33200000000000002</v>
       </c>
-    </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I55" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72500000000000009</v>
+      </c>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>55</v>
       </c>
@@ -2088,8 +2391,12 @@
       <c r="G56" s="1">
         <v>0.314</v>
       </c>
-    </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I56" s="1">
+        <f t="shared" si="0"/>
+        <v>0.7360000000000001</v>
+      </c>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>56</v>
       </c>
@@ -2111,8 +2418,12 @@
       <c r="G57" s="1">
         <v>0.26900000000000002</v>
       </c>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I57" s="1">
+        <f t="shared" si="0"/>
+        <v>0.74199999999999999</v>
+      </c>
+    </row>
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>57</v>
       </c>
@@ -2134,8 +2445,12 @@
       <c r="G58" s="1">
         <v>0.36299999999999999</v>
       </c>
-    </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I58" s="1">
+        <f t="shared" si="0"/>
+        <v>0.75600000000000001</v>
+      </c>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>58</v>
       </c>
@@ -2157,8 +2472,12 @@
       <c r="G59" s="1">
         <v>0.32900000000000001</v>
       </c>
-    </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I59" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71500000000000008</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>59</v>
       </c>
@@ -2180,8 +2499,12 @@
       <c r="G60" s="1">
         <v>0.432</v>
       </c>
-    </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I60" s="1">
+        <f t="shared" si="0"/>
+        <v>0.71799999999999997</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>60</v>
       </c>
@@ -2203,8 +2526,12 @@
       <c r="G61" s="1">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I61" s="1">
+        <f t="shared" si="0"/>
+        <v>0.7320000000000001</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>61</v>
       </c>
@@ -2226,8 +2553,12 @@
       <c r="G62" s="1">
         <v>0.35199999999999998</v>
       </c>
-    </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I62" s="1">
+        <f t="shared" si="0"/>
+        <v>0.69400000000000006</v>
+      </c>
+    </row>
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>62</v>
       </c>
@@ -2249,8 +2580,12 @@
       <c r="G63" s="1">
         <v>0.378</v>
       </c>
-    </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I63" s="1">
+        <f t="shared" si="0"/>
+        <v>0.73299999999999998</v>
+      </c>
+    </row>
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>63</v>
       </c>
@@ -2272,8 +2607,12 @@
       <c r="G64" s="1">
         <v>0.29599999999999999</v>
       </c>
-    </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I64" s="1">
+        <f t="shared" si="0"/>
+        <v>0.72799999999999998</v>
+      </c>
+    </row>
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>64</v>
       </c>
@@ -2295,8 +2634,12 @@
       <c r="G65" s="1">
         <v>0.39700000000000002</v>
       </c>
-    </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I65" s="1">
+        <f t="shared" si="0"/>
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>65</v>
       </c>
@@ -2318,8 +2661,12 @@
       <c r="G66" s="1">
         <v>0.377</v>
       </c>
-    </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I66" s="1">
+        <f t="shared" si="0"/>
+        <v>0.69600000000000006</v>
+      </c>
+    </row>
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>66</v>
       </c>
@@ -2341,8 +2688,12 @@
       <c r="G67" s="1">
         <v>0.40500000000000003</v>
       </c>
-    </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I67" s="1">
+        <f t="shared" ref="I67:I130" si="1">SUM(B67:D67)</f>
+        <v>0.70600000000000007</v>
+      </c>
+    </row>
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>67</v>
       </c>
@@ -2364,8 +2715,12 @@
       <c r="G68" s="1">
         <v>0.26100000000000001</v>
       </c>
-    </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I68" s="1">
+        <f t="shared" si="1"/>
+        <v>0.748</v>
+      </c>
+    </row>
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>68</v>
       </c>
@@ -2387,8 +2742,12 @@
       <c r="G69" s="1">
         <v>0.29499999999999998</v>
       </c>
-    </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I69" s="1">
+        <f t="shared" si="1"/>
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>69</v>
       </c>
@@ -2410,8 +2769,12 @@
       <c r="G70" s="1">
         <v>0.39400000000000002</v>
       </c>
-    </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I70" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77800000000000002</v>
+      </c>
+    </row>
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>70</v>
       </c>
@@ -2433,8 +2796,12 @@
       <c r="G71" s="1">
         <v>0.28199999999999997</v>
       </c>
-    </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I71" s="1">
+        <f t="shared" si="1"/>
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>71</v>
       </c>
@@ -2456,8 +2823,12 @@
       <c r="G72" s="1">
         <v>0.28899999999999998</v>
       </c>
-    </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I72" s="1">
+        <f t="shared" si="1"/>
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>72</v>
       </c>
@@ -2479,8 +2850,12 @@
       <c r="G73" s="1">
         <v>0.28399999999999997</v>
       </c>
-    </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I73" s="1">
+        <f t="shared" si="1"/>
+        <v>0.73399999999999999</v>
+      </c>
+    </row>
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>73</v>
       </c>
@@ -2502,8 +2877,12 @@
       <c r="G74" s="1">
         <v>0.30599999999999999</v>
       </c>
-    </row>
-    <row r="75" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I74" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
         <v>74</v>
       </c>
@@ -2525,8 +2904,12 @@
       <c r="G75" s="1">
         <v>0.27500000000000002</v>
       </c>
-    </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I75" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79500000000000004</v>
+      </c>
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -2548,8 +2931,12 @@
       <c r="G76" s="1">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I76" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -2571,8 +2958,12 @@
       <c r="G77" s="1">
         <v>0.31900000000000001</v>
       </c>
-    </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I77" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -2594,8 +2985,12 @@
       <c r="G78" s="1">
         <v>0.34899999999999998</v>
       </c>
-    </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I78" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -2617,8 +3012,12 @@
       <c r="G79" s="1">
         <v>0.35699999999999998</v>
       </c>
-    </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I79" s="1">
+        <f t="shared" si="1"/>
+        <v>0.876</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -2640,8 +3039,12 @@
       <c r="G80" s="1">
         <v>0.34200000000000003</v>
       </c>
-    </row>
-    <row r="81" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I80" s="1">
+        <f t="shared" si="1"/>
+        <v>0.749</v>
+      </c>
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -2663,8 +3066,12 @@
       <c r="G81" s="1">
         <v>0.41</v>
       </c>
-    </row>
-    <row r="82" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I81" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78300000000000003</v>
+      </c>
+    </row>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2686,8 +3093,12 @@
       <c r="G82" s="1">
         <v>0.33700000000000002</v>
       </c>
-    </row>
-    <row r="83" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I82" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2709,8 +3120,12 @@
       <c r="G83" s="1">
         <v>0.32</v>
       </c>
-    </row>
-    <row r="84" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I83" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2732,8 +3147,12 @@
       <c r="G84" s="1">
         <v>0.40200000000000002</v>
       </c>
-    </row>
-    <row r="85" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I84" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79300000000000004</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2755,8 +3174,12 @@
       <c r="G85" s="1">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="86" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I85" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81899999999999995</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2778,8 +3201,12 @@
       <c r="G86" s="1">
         <v>0.312</v>
       </c>
-    </row>
-    <row r="87" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I86" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2801,8 +3228,12 @@
       <c r="G87" s="1">
         <v>0.33600000000000002</v>
       </c>
-    </row>
-    <row r="88" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I87" s="1">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2824,8 +3255,12 @@
       <c r="G88" s="1">
         <v>0.36399999999999999</v>
       </c>
-    </row>
-    <row r="89" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I88" s="1">
+        <f t="shared" si="1"/>
+        <v>0.75800000000000001</v>
+      </c>
+    </row>
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2847,8 +3282,12 @@
       <c r="G89" s="1">
         <v>0.27700000000000002</v>
       </c>
-    </row>
-    <row r="90" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I89" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2870,8 +3309,12 @@
       <c r="G90" s="1">
         <v>0.35299999999999998</v>
       </c>
-    </row>
-    <row r="91" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I90" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2893,8 +3336,12 @@
       <c r="G91" s="1">
         <v>0.34200000000000003</v>
       </c>
-    </row>
-    <row r="92" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I91" s="1">
+        <f t="shared" si="1"/>
+        <v>0.753</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2916,8 +3363,12 @@
       <c r="G92" s="1">
         <v>0.318</v>
       </c>
-    </row>
-    <row r="93" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I92" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2939,8 +3390,12 @@
       <c r="G93" s="1">
         <v>0.31900000000000001</v>
       </c>
-    </row>
-    <row r="94" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I93" s="1">
+        <f t="shared" si="1"/>
+        <v>0.75900000000000001</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2962,8 +3417,12 @@
       <c r="G94" s="1">
         <v>0.40300000000000002</v>
       </c>
-    </row>
-    <row r="95" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I94" s="1">
+        <f t="shared" si="1"/>
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" t="s">
         <v>94</v>
       </c>
@@ -2985,8 +3444,12 @@
       <c r="G95" s="1">
         <v>0.27900000000000003</v>
       </c>
-    </row>
-    <row r="96" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I95" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>95</v>
       </c>
@@ -3008,8 +3471,12 @@
       <c r="G96" s="1">
         <v>0.32100000000000001</v>
       </c>
-    </row>
-    <row r="97" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I96" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79900000000000004</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>96</v>
       </c>
@@ -3031,8 +3498,12 @@
       <c r="G97" s="1">
         <v>0.32200000000000001</v>
       </c>
-    </row>
-    <row r="98" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I97" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89800000000000002</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>97</v>
       </c>
@@ -3054,8 +3525,12 @@
       <c r="G98" s="1">
         <v>0.27900000000000003</v>
       </c>
-    </row>
-    <row r="99" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I98" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>98</v>
       </c>
@@ -3077,8 +3552,12 @@
       <c r="G99" s="1">
         <v>0.27400000000000002</v>
       </c>
-    </row>
-    <row r="100" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I99" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" t="s">
         <v>99</v>
       </c>
@@ -3100,8 +3579,12 @@
       <c r="G100" s="1">
         <v>0.29099999999999998</v>
       </c>
-    </row>
-    <row r="101" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I100" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>100</v>
       </c>
@@ -3123,8 +3606,12 @@
       <c r="G101" s="1">
         <v>0.28599999999999998</v>
       </c>
-    </row>
-    <row r="102" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I101" s="1">
+        <f t="shared" si="1"/>
+        <v>0.73599999999999999</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>101</v>
       </c>
@@ -3146,8 +3633,12 @@
       <c r="G102" s="1">
         <v>0.33500000000000002</v>
       </c>
-    </row>
-    <row r="103" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I102" s="1">
+        <f t="shared" si="1"/>
+        <v>0.747</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" t="s">
         <v>102</v>
       </c>
@@ -3169,8 +3660,12 @@
       <c r="G103" s="1">
         <v>0.34699999999999998</v>
       </c>
-    </row>
-    <row r="104" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I103" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78900000000000003</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>103</v>
       </c>
@@ -3192,8 +3687,12 @@
       <c r="G104" s="1">
         <v>0.27900000000000003</v>
       </c>
-    </row>
-    <row r="105" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I104" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" t="s">
         <v>104</v>
       </c>
@@ -3215,8 +3714,12 @@
       <c r="G105" s="1">
         <v>0.25900000000000001</v>
       </c>
-    </row>
-    <row r="106" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I105" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76600000000000001</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>105</v>
       </c>
@@ -3238,8 +3741,12 @@
       <c r="G106" s="1">
         <v>0.30199999999999999</v>
       </c>
-    </row>
-    <row r="107" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I106" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>106</v>
       </c>
@@ -3261,8 +3768,12 @@
       <c r="G107" s="1">
         <v>0.23200000000000001</v>
       </c>
-    </row>
-    <row r="108" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I107" s="1">
+        <f t="shared" si="1"/>
+        <v>0.745</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>107</v>
       </c>
@@ -3284,8 +3795,12 @@
       <c r="G108" s="1">
         <v>0.29399999999999998</v>
       </c>
-    </row>
-    <row r="109" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I108" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77200000000000002</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>108</v>
       </c>
@@ -3307,8 +3822,12 @@
       <c r="G109" s="1">
         <v>0.27200000000000002</v>
       </c>
-    </row>
-    <row r="110" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I109" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>109</v>
       </c>
@@ -3330,8 +3849,12 @@
       <c r="G110" s="1">
         <v>0.27100000000000002</v>
       </c>
-    </row>
-    <row r="111" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I110" s="1">
+        <f t="shared" si="1"/>
+        <v>0.80800000000000005</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>110</v>
       </c>
@@ -3353,8 +3876,12 @@
       <c r="G111" s="1">
         <v>0.27100000000000002</v>
       </c>
-    </row>
-    <row r="112" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I111" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>111</v>
       </c>
@@ -3376,8 +3903,12 @@
       <c r="G112" s="1">
         <v>0.25800000000000001</v>
       </c>
-    </row>
-    <row r="113" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I112" s="1">
+        <f t="shared" si="1"/>
+        <v>0.83899999999999997</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>112</v>
       </c>
@@ -3399,8 +3930,12 @@
       <c r="G113" s="1">
         <v>0.309</v>
       </c>
-    </row>
-    <row r="114" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I113" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77100000000000002</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>113</v>
       </c>
@@ -3422,8 +3957,12 @@
       <c r="G114" s="1">
         <v>0.27100000000000002</v>
       </c>
-    </row>
-    <row r="115" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I114" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>114</v>
       </c>
@@ -3445,8 +3984,12 @@
       <c r="G115" s="1">
         <v>0.24</v>
       </c>
-    </row>
-    <row r="116" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I115" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>115</v>
       </c>
@@ -3468,8 +4011,12 @@
       <c r="G116" s="1">
         <v>0.29399999999999998</v>
       </c>
-    </row>
-    <row r="117" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I116" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>116</v>
       </c>
@@ -3491,8 +4038,12 @@
       <c r="G117" s="1">
         <v>0.252</v>
       </c>
-    </row>
-    <row r="118" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I117" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>117</v>
       </c>
@@ -3514,8 +4065,12 @@
       <c r="G118" s="1">
         <v>0.27900000000000003</v>
       </c>
-    </row>
-    <row r="119" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I118" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>118</v>
       </c>
@@ -3537,8 +4092,12 @@
       <c r="G119" s="1">
         <v>0.25900000000000001</v>
       </c>
-    </row>
-    <row r="120" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I119" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>119</v>
       </c>
@@ -3560,8 +4119,12 @@
       <c r="G120" s="1">
         <v>0.40600000000000003</v>
       </c>
-    </row>
-    <row r="121" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I120" s="1">
+        <f t="shared" si="1"/>
+        <v>0.78100000000000003</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>120</v>
       </c>
@@ -3583,8 +4146,12 @@
       <c r="G121" s="1">
         <v>0.33700000000000002</v>
       </c>
-    </row>
-    <row r="122" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I121" s="1">
+        <f t="shared" si="1"/>
+        <v>0.77300000000000002</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>121</v>
       </c>
@@ -3606,8 +4173,12 @@
       <c r="G122" s="1">
         <v>0.34899999999999998</v>
       </c>
-    </row>
-    <row r="123" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I122" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76200000000000001</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>122</v>
       </c>
@@ -3629,8 +4200,12 @@
       <c r="G123" s="1">
         <v>0.28399999999999997</v>
       </c>
-    </row>
-    <row r="124" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I123" s="1">
+        <f t="shared" si="1"/>
+        <v>0.79300000000000004</v>
+      </c>
+    </row>
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>123</v>
       </c>
@@ -3652,8 +4227,12 @@
       <c r="G124" s="1">
         <v>0.27600000000000002</v>
       </c>
-    </row>
-    <row r="125" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I124" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>124</v>
       </c>
@@ -3675,8 +4254,12 @@
       <c r="G125" s="1">
         <v>0.30499999999999999</v>
       </c>
-    </row>
-    <row r="126" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I125" s="1">
+        <f t="shared" si="1"/>
+        <v>0.81800000000000006</v>
+      </c>
+    </row>
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126" t="s">
         <v>125</v>
       </c>
@@ -3698,8 +4281,12 @@
       <c r="G126" s="1">
         <v>0.29399999999999998</v>
       </c>
-    </row>
-    <row r="127" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I126" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76900000000000002</v>
+      </c>
+    </row>
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>126</v>
       </c>
@@ -3721,8 +4308,12 @@
       <c r="G127" s="1">
         <v>0.25900000000000001</v>
       </c>
-    </row>
-    <row r="128" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I127" s="1">
+        <f t="shared" si="1"/>
+        <v>0.73899999999999999</v>
+      </c>
+    </row>
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>127</v>
       </c>
@@ -3744,8 +4335,12 @@
       <c r="G128" s="1">
         <v>0.41199999999999998</v>
       </c>
-    </row>
-    <row r="129" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I128" s="1">
+        <f t="shared" si="1"/>
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="129" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>128</v>
       </c>
@@ -3767,8 +4362,12 @@
       <c r="G129" s="1">
         <v>0.38100000000000001</v>
       </c>
-    </row>
-    <row r="130" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I129" s="1">
+        <f t="shared" si="1"/>
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="130" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>129</v>
       </c>
@@ -3790,8 +4389,12 @@
       <c r="G130" s="1">
         <v>0.32700000000000001</v>
       </c>
-    </row>
-    <row r="131" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I130" s="1">
+        <f t="shared" si="1"/>
+        <v>0.82000000000000006</v>
+      </c>
+    </row>
+    <row r="131" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>130</v>
       </c>
@@ -3813,8 +4416,12 @@
       <c r="G131" s="1">
         <v>0.32100000000000001</v>
       </c>
-    </row>
-    <row r="132" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I131" s="1">
+        <f t="shared" ref="I131:I141" si="2">SUM(B131:D131)</f>
+        <v>0.77900000000000003</v>
+      </c>
+    </row>
+    <row r="132" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>131</v>
       </c>
@@ -3836,8 +4443,12 @@
       <c r="G132" s="1">
         <v>0.309</v>
       </c>
-    </row>
-    <row r="133" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I132" s="1">
+        <f t="shared" si="2"/>
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="133" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>132</v>
       </c>
@@ -3859,8 +4470,12 @@
       <c r="G133" s="1">
         <v>0.313</v>
       </c>
-    </row>
-    <row r="134" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I133" s="1">
+        <f t="shared" si="2"/>
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="134" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>133</v>
       </c>
@@ -3882,8 +4497,12 @@
       <c r="G134" s="1">
         <v>0.318</v>
       </c>
-    </row>
-    <row r="135" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I134" s="1">
+        <f t="shared" si="2"/>
+        <v>0.76100000000000001</v>
+      </c>
+    </row>
+    <row r="135" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>134</v>
       </c>
@@ -3905,8 +4524,12 @@
       <c r="G135" s="1">
         <v>0.29199999999999998</v>
       </c>
-    </row>
-    <row r="136" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I135" s="1">
+        <f t="shared" si="2"/>
+        <v>0.79400000000000004</v>
+      </c>
+    </row>
+    <row r="136" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>135</v>
       </c>
@@ -3928,8 +4551,12 @@
       <c r="G136" s="1">
         <v>0.312</v>
       </c>
-    </row>
-    <row r="137" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I136" s="1">
+        <f t="shared" si="2"/>
+        <v>0.79300000000000004</v>
+      </c>
+    </row>
+    <row r="137" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>136</v>
       </c>
@@ -3951,8 +4578,12 @@
       <c r="G137" s="1">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="138" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I137" s="1">
+        <f t="shared" si="2"/>
+        <v>0.754</v>
+      </c>
+    </row>
+    <row r="138" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>137</v>
       </c>
@@ -3974,8 +4605,12 @@
       <c r="G138" s="1">
         <v>0.28599999999999998</v>
       </c>
-    </row>
-    <row r="139" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I138" s="1">
+        <f t="shared" si="2"/>
+        <v>0.76800000000000002</v>
+      </c>
+    </row>
+    <row r="139" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>138</v>
       </c>
@@ -3997,8 +4632,12 @@
       <c r="G139" s="1">
         <v>0.307</v>
       </c>
-    </row>
-    <row r="140" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I139" s="1">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="140" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>139</v>
       </c>
@@ -4020,8 +4659,12 @@
       <c r="G140" s="1">
         <v>0.29899999999999999</v>
       </c>
-    </row>
-    <row r="141" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="I140" s="1">
+        <f t="shared" si="2"/>
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="141" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>140</v>
       </c>
@@ -4043,8 +4686,15 @@
       <c r="G141" s="1">
         <v>0.27600000000000002</v>
       </c>
+      <c r="I141" s="1">
+        <f t="shared" si="2"/>
+        <v>0.73599999999999999</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <ignoredErrors>
+    <ignoredError sqref="I2" formulaRange="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>